<commit_message>
round 23.5-cm T56 offset up instead of down
</commit_message>
<xml_diff>
--- a/rawdata/rhizotube-offsets.xlsx
+++ b/rawdata/rhizotube-offsets.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="620" yWindow="20" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -416,14 +416,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -456,7 +450,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -465,90 +459,90 @@
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -579,7 +573,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -902,14 +896,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.5703125" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
@@ -1320,7 +1314,7 @@
         <v>56</v>
       </c>
       <c r="O10" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P10" s="2"/>
     </row>
@@ -3057,7 +3051,7 @@
   <pageMargins left="0.75" right="0.75" top="0.59722222222222221" bottom="0.61111111111111116" header="0.59722222222222221" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>